<commit_message>
shortened init baseline to tblshting
shortened from 16 to 2 s for troubleshooting; need to change back
</commit_message>
<xml_diff>
--- a/Experiment/Orders_LOC/PAR01_RUN01.xlsx
+++ b/Experiment/Orders_LOC/PAR01_RUN01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VisionLab\AppData\Local\GitHubDesktop\app-2.9.0\fMRI_3DFaces_MD_2021\Experiment\Orders_LOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A1C35A-2EAC-4C11-8469-5CA696BA5FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305DC88B-4C2C-457A-BB52-CED1EF902588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -571,7 +571,7 @@
   <dimension ref="A1:F266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L79" sqref="L79"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,7 +608,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>

</xml_diff>